<commit_message>
Se modifica builder para insertar los datos de la prueba
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Trn_0369Autenticacion.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Trn_0369Autenticacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariaMartinez/Documents/Repositorios/AW1059001_NuevaAPPSucursalVirtualPersonas_Test/APP_PERSONAS/src/test/resources/datadriven/autenticacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA99FD2D-8DB2-044E-816F-C71F03C68CDA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CFCFB6-1926-C447-AE3E-4C31D62917D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16920" yWindow="0" windowWidth="16680" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -112,21 +112,12 @@
     <t>segundaClave</t>
   </si>
   <si>
-    <t>jacinto25</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
     <t>1037655531</t>
   </si>
   <si>
-    <t>1223</t>
-  </si>
-  <si>
-    <t>3221</t>
-  </si>
-  <si>
     <t>0369</t>
   </si>
   <si>
@@ -143,6 +134,15 @@
   </si>
   <si>
     <t>ACTIVO</t>
+  </si>
+  <si>
+    <t>seguridad01</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>4321</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -590,30 +590,30 @@
         <v>3</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>4</v>
@@ -622,16 +622,16 @@
         <v>5</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="L2" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizacion mapeo, inicio registro
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Trn_0369Autenticacion.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Trn_0369Autenticacion.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -143,13 +143,28 @@
   </si>
   <si>
     <t>1111</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>95400152</t>
+  </si>
+  <si>
+    <t>sandrita69</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>0370</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -169,6 +184,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -220,7 +242,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -228,6 +250,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -517,7 +540,7 @@
     <col min="9" max="9" width="18.375" customWidth="1"/>
     <col min="10" max="10" width="22.125" customWidth="1"/>
     <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="12" max="12" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -634,17 +657,55 @@
         <v>22</v>
       </c>
     </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:J3</xm:sqref>
+          <xm:sqref>G2:J4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Se agregan nuevas clases de integracion
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Trn_0369Autenticacion.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Trn_0369Autenticacion.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\OSP_NEW\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\autenticacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AUTOMATIZACION JAVA\PROYECTOS GRADLE\PROYECTOS NUEVA APP\AW1059001_APPSucursalVirtualPersonas_Test\APP_PERSONAS\src\test\resources\datadriven\autenticacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -158,12 +158,21 @@
   </si>
   <si>
     <t>0370</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>58156994</t>
+  </si>
+  <si>
+    <t>invictus01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="12"/>
@@ -242,15 +251,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,20 +537,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.125" style="6" customWidth="1"/>
+    <col min="2" max="6" width="14.375" style="6" customWidth="1"/>
+    <col min="7" max="8" width="11" style="6"/>
+    <col min="9" max="9" width="18.375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="22.125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="14.375" style="6" customWidth="1"/>
+    <col min="12" max="12" width="14.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="11" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -582,22 +594,22 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -612,30 +624,30 @@
       <c r="J2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -650,48 +662,86 @@
       <c r="J3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>22</v>
       </c>
     </row>
@@ -705,7 +755,7 @@
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:J4</xm:sqref>
+          <xm:sqref>G2:J5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>